<commit_message>
Triangulated objs, re-exported with Bounding Boxes
</commit_message>
<xml_diff>
--- a/Assignment 2/DirectX11/Project Rubric.xlsx
+++ b/Assignment 2/DirectX11/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c385a0523d84e/Documents/Full Sail/3D Content Creation/3dcc-course-materials-CodeWithJazmine/Assignment 2/DirectX11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DFC2E6A-A2D3-408D-BCC0-9F504B498C24}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45EAD454-CFB3-4E56-8437-7F4DCACF5154}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -2061,6 +2061,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2360,8 +2364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2962,7 @@
         <v>0.03</v>
       </c>
       <c r="C52" s="3">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2985,7 +2989,7 @@
       </c>
       <c r="C54" s="13">
         <f>SUM(C51:C53)</f>
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2998,7 +3002,7 @@
       </c>
       <c r="C55" s="16">
         <f>MIN(SUM(C54,C49,C29,C12),100%)</f>
-        <v>0.6</v>
+        <v>0.62999999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Music and SFX added
SFX plays when camera switches (when 'C' is pressed)
</commit_message>
<xml_diff>
--- a/Assignment 2/DirectX11/Project Rubric.xlsx
+++ b/Assignment 2/DirectX11/Project Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c385a0523d84e/Documents/Full Sail/3D Content Creation/3dcc-course-materials-CodeWithJazmine/Assignment 2/DirectX11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5842EF8B-01F1-40EC-A13D-420E360A4296}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC5DC224-FF6C-40A2-9820-D358BAECE3A2}"/>
   <bookViews>
-    <workbookView xWindow="11295" yWindow="1860" windowWidth="19110" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="0" yWindow="2790" windowWidth="21315" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1539,7 +1539,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1703,7 +1703,7 @@
     <t>Fully complete 7 or more Key Features</t>
   </si>
   <si>
-    <t>I want to do this</t>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -2364,8 +2364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,9 +2529,6 @@
       <c r="C14" s="3">
         <v>0.05</v>
       </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
@@ -2541,7 +2538,10 @@
         <v>0.05</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>0.02</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="C29" s="6">
         <f>MIN(SUM(C14:C28),33%)</f>
-        <v>0.1</v>
+        <v>0.12000000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2948,7 +2948,7 @@
         <v>0.03</v>
       </c>
       <c r="C51" s="3">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="D51" t="s">
         <v>54</v>
@@ -2975,9 +2975,6 @@
       <c r="C53" s="7">
         <v>0</v>
       </c>
-      <c r="D53" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
@@ -2989,7 +2986,7 @@
       </c>
       <c r="C54" s="13">
         <f>SUM(C51:C53)</f>
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -3002,7 +2999,7 @@
       </c>
       <c r="C55" s="16">
         <f>MIN(SUM(C54,C49,C29,C12),100%)</f>
-        <v>0.62999999999999989</v>
+        <v>0.67999999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Level Renderer Project Submitted
</commit_message>
<xml_diff>
--- a/Assignment 2/DirectX11/Project Rubric.xlsx
+++ b/Assignment 2/DirectX11/Project Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c385a0523d84e/Documents/Full Sail/3D Content Creation/3dcc-course-materials-CodeWithJazmine/Assignment 2/DirectX11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC5DC224-FF6C-40A2-9820-D358BAECE3A2}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3E4E466-9BC6-4EF8-AC67-81CB288C3794}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2790" windowWidth="21315" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="13140" yWindow="930" windowWidth="21315" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2364,8 +2364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>